<commit_message>
Table S2 comments compared to Jimmy (we need also elevation lienar effects to tets for + looks Jimmy set up of beta bin. models converged muhc better for Tanzania), probably better to go for Jimmy package and set up unless really good reason, why not to do so (otherwise results withh be the same/similar, if we stay with practise reporting also singificancies for models via LR test that are very close to null = similar good).
</commit_message>
<xml_diff>
--- a/Outputs/Table_S2_models-pk.xlsx
+++ b/Outputs/Table_S2_models-pk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="47">
   <si>
     <t>regions</t>
   </si>
@@ -142,12 +142,36 @@
   <si>
     <t>not sign. as elevation1 not tested</t>
   </si>
+  <si>
+    <t>newly marginal (decline perhaps)</t>
+  </si>
+  <si>
+    <t>similar (in Jimmy code elevation1 better)</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>marginal, the same / in Jimmy we still plotted trends the same god as null model and within 0.1 p</t>
+  </si>
+  <si>
+    <t>similar (was p value 0.048, now 0.05 could be still sign?)</t>
+  </si>
+  <si>
+    <t>elevation1 was sign.</t>
+  </si>
+  <si>
+    <t>elevation1 was sign, Jimmy models muhc better convergence!</t>
+  </si>
+  <si>
+    <t>elevation1 was sign, Jimmy models much better convergence!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +182,32 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -197,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -212,6 +262,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,11 +557,12 @@
   <dimension ref="A2:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="60.625" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="24.375" customWidth="1"/>
     <col min="4" max="4" width="19.75" customWidth="1"/>
@@ -678,62 +741,62 @@
       </c>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:21" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:21" s="6" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="7">
         <v>66.55</v>
       </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
         <v>0.78</v>
       </c>
-      <c r="I5" s="2" t="b">
+      <c r="I5" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="7">
         <v>3</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="7">
         <v>65.290000000000006</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="7">
         <v>68.69</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="7">
         <v>-29.64</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="7">
         <v>59.29</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="7">
         <v>9.41</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="7">
         <v>1</v>
       </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="s">
+      <c r="S5" s="7">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1085,68 +1148,68 @@
       </c>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:21" s="5" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:21" s="8" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="9">
         <v>7</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="9">
         <v>81.5</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="9">
         <v>5.3</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="9">
         <v>0.04</v>
       </c>
-      <c r="I12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="I12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
         <v>0.02</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="4">
+      <c r="K12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="9">
         <v>7</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="9">
         <v>74.040000000000006</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="9">
         <v>81.98</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="9">
         <v>-30.02</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="9">
         <v>60.04</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="9">
         <v>12.75</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="9">
         <v>5</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="9">
         <v>0.03</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="T12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="U12" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1207,62 +1270,65 @@
       </c>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:21" s="5" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>4</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>79.48</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="4">
         <v>0.36</v>
       </c>
-      <c r="I14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
         <v>0.01</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="K14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="4">
         <v>4</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="4">
         <v>77.260000000000005</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="4">
         <v>81.8</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="4">
         <v>-34.630000000000003</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="4">
         <v>69.260000000000005</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="4">
         <v>5.33</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="4">
         <v>2</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="T14" s="2"/>
+      <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:21" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1378,7 +1444,7 @@
       </c>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1435,7 +1501,7 @@
       </c>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +1558,7 @@
       </c>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1549,7 +1615,7 @@
       </c>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1606,7 +1672,7 @@
       </c>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1663,7 +1729,7 @@
       </c>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1720,7 +1786,7 @@
       </c>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1777,66 +1843,69 @@
       </c>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:20" s="6" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="7">
         <v>4</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="7">
         <v>70.56</v>
       </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24" s="7">
         <v>0.82</v>
       </c>
-      <c r="I24" s="2" t="b">
+      <c r="I24" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="2">
+      <c r="J24" s="7">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="7">
         <v>4</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="7">
         <v>68.34</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="7">
         <v>72.88</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="7">
         <v>-30.17</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="7">
         <v>60.34</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="Q24" s="7">
         <v>16.690000000000001</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24" s="7">
         <v>2</v>
       </c>
-      <c r="S24" s="2">
-        <v>0</v>
-      </c>
-      <c r="T24" s="2" t="s">
+      <c r="S24" s="7">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -1893,7 +1962,7 @@
       </c>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1952,7 +2021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2011,7 +2080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2137,7 @@
       </c>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
@@ -2125,66 +2194,69 @@
       </c>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="1:20" s="6" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="7">
         <v>3</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="7">
         <v>79.37</v>
       </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7">
         <v>0.82</v>
       </c>
-      <c r="I30" s="2" t="b">
+      <c r="I30" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="7">
         <v>0.27</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="2">
+      <c r="K30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="7">
         <v>3</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="7">
         <v>78.11</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="7">
         <v>81.510000000000005</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="7">
         <v>-36.049999999999997</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="7">
         <v>72.11</v>
       </c>
-      <c r="Q30" s="2">
+      <c r="Q30" s="7">
         <v>6.69</v>
       </c>
-      <c r="R30" s="2">
+      <c r="R30" s="7">
         <v>1</v>
       </c>
-      <c r="S30" s="2">
+      <c r="S30" s="7">
         <v>0.01</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="T30" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>19</v>
       </c>
@@ -2241,7 +2313,7 @@
       </c>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
@@ -2300,7 +2372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
@@ -2357,7 +2429,7 @@
       </c>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
@@ -2414,66 +2486,69 @@
       </c>
       <c r="T34" s="2"/>
     </row>
-    <row r="35" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="1:20" s="6" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="7">
         <v>3</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="7">
         <v>64.66</v>
       </c>
-      <c r="G35" s="2">
-        <v>0</v>
-      </c>
-      <c r="H35" s="2">
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
         <v>0.91</v>
       </c>
-      <c r="I35" s="2" t="b">
+      <c r="I35" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="7">
         <v>0.03</v>
       </c>
-      <c r="K35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L35" s="2">
+      <c r="K35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" s="7">
         <v>3</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35" s="7">
         <v>63.16</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="7">
         <v>66.150000000000006</v>
       </c>
-      <c r="O35" s="2">
+      <c r="O35" s="7">
         <v>-28.58</v>
       </c>
-      <c r="P35" s="2">
+      <c r="P35" s="7">
         <v>57.16</v>
       </c>
-      <c r="Q35" s="2">
+      <c r="Q35" s="7">
         <v>8.58</v>
       </c>
-      <c r="R35" s="2">
+      <c r="R35" s="7">
         <v>1</v>
       </c>
-      <c r="S35" s="2">
-        <v>0</v>
-      </c>
-      <c r="T35" s="2" t="s">
+      <c r="S35" s="7">
+        <v>0</v>
+      </c>
+      <c r="T35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2532,7 +2607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2589,7 +2664,7 @@
       </c>
       <c r="T37" s="2"/>
     </row>
-    <row r="38" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
@@ -2646,7 +2721,7 @@
       </c>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
@@ -2703,7 +2778,7 @@
       </c>
       <c r="T39" s="2"/>
     </row>
-    <row r="40" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>35</v>
       </c>
@@ -2760,7 +2835,7 @@
       </c>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>35</v>
       </c>
@@ -2817,7 +2892,7 @@
       </c>
       <c r="T41" s="2"/>
     </row>
-    <row r="42" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>35</v>
       </c>
@@ -2874,7 +2949,7 @@
       </c>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>35</v>
       </c>
@@ -2931,7 +3006,7 @@
       </c>
       <c r="T43" s="2"/>
     </row>
-    <row r="44" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>35</v>
       </c>
@@ -2988,64 +3063,67 @@
       </c>
       <c r="T44" s="2"/>
     </row>
-    <row r="45" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
+    <row r="45" spans="1:20" s="6" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="7">
         <v>3</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="7">
         <v>72.790000000000006</v>
       </c>
-      <c r="G45" s="2">
-        <v>0</v>
-      </c>
-      <c r="H45" s="2">
+      <c r="G45" s="7">
+        <v>0</v>
+      </c>
+      <c r="H45" s="7">
         <v>0.54</v>
       </c>
-      <c r="I45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2">
-        <v>0</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L45" s="2">
+      <c r="I45" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="7">
+        <v>0</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" s="7">
         <v>3</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="7">
         <v>71.290000000000006</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="7">
         <v>74.28</v>
       </c>
-      <c r="O45" s="2">
+      <c r="O45" s="7">
         <v>-32.64</v>
       </c>
-      <c r="P45" s="2">
+      <c r="P45" s="7">
         <v>65.290000000000006</v>
       </c>
-      <c r="Q45" s="2">
+      <c r="Q45" s="7">
         <v>3.58</v>
       </c>
-      <c r="R45" s="2">
+      <c r="R45" s="7">
         <v>1</v>
       </c>
-      <c r="S45" s="2">
+      <c r="S45" s="7">
         <v>0.06</v>
       </c>
-      <c r="T45" s="2"/>
-    </row>
-    <row r="46" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="T45" s="7"/>
+    </row>
+    <row r="46" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>35</v>
       </c>
@@ -3102,7 +3180,7 @@
       </c>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>35</v>
       </c>
@@ -3159,7 +3237,7 @@
       </c>
       <c r="T47" s="2"/>
     </row>
-    <row r="48" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>35</v>
       </c>
@@ -3216,7 +3294,7 @@
       </c>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>35</v>
       </c>
@@ -3273,7 +3351,7 @@
       </c>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>35</v>
       </c>
@@ -3330,7 +3408,7 @@
       </c>
       <c r="T50" s="2"/>
     </row>
-    <row r="51" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>35</v>
       </c>
@@ -3387,7 +3465,7 @@
       </c>
       <c r="T51" s="2"/>
     </row>
-    <row r="52" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>35</v>
       </c>
@@ -3444,7 +3522,7 @@
       </c>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>35</v>
       </c>
@@ -3501,7 +3579,7 @@
       </c>
       <c r="T53" s="2"/>
     </row>
-    <row r="54" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>35</v>
       </c>
@@ -3558,7 +3636,7 @@
       </c>
       <c r="T54" s="2"/>
     </row>
-    <row r="55" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>35</v>
       </c>
@@ -3617,7 +3695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>35</v>
       </c>
@@ -3676,7 +3754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>35</v>
       </c>
@@ -3733,7 +3811,7 @@
       </c>
       <c r="T57" s="2"/>
     </row>
-    <row r="58" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>35</v>
       </c>
@@ -3790,7 +3868,7 @@
       </c>
       <c r="T58" s="2"/>
     </row>
-    <row r="59" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>35</v>
       </c>
@@ -3847,66 +3925,69 @@
       </c>
       <c r="T59" s="2"/>
     </row>
-    <row r="60" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
+    <row r="60" spans="1:20" s="6" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="7">
         <v>3</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="7">
         <v>73.900000000000006</v>
       </c>
-      <c r="G60" s="2">
-        <v>0</v>
-      </c>
-      <c r="H60" s="2">
+      <c r="G60" s="7">
+        <v>0</v>
+      </c>
+      <c r="H60" s="7">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I60" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J60" s="2">
-        <v>0</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L60" s="2">
+      <c r="I60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" s="7">
+        <v>0</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L60" s="7">
         <v>3</v>
       </c>
-      <c r="M60" s="2">
+      <c r="M60" s="7">
         <v>72.400000000000006</v>
       </c>
-      <c r="N60" s="2">
+      <c r="N60" s="7">
         <v>75.39</v>
       </c>
-      <c r="O60" s="2">
+      <c r="O60" s="7">
         <v>-33.200000000000003</v>
       </c>
-      <c r="P60" s="2">
+      <c r="P60" s="7">
         <v>66.400000000000006</v>
       </c>
-      <c r="Q60" s="2">
+      <c r="Q60" s="7">
         <v>3.9</v>
       </c>
-      <c r="R60" s="2">
+      <c r="R60" s="7">
         <v>1</v>
       </c>
-      <c r="S60" s="2">
+      <c r="S60" s="7">
         <v>0.05</v>
       </c>
-      <c r="T60" s="2" t="s">
+      <c r="T60" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>35</v>
       </c>
@@ -3963,7 +4044,7 @@
       </c>
       <c r="T61" s="2"/>
     </row>
-    <row r="62" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>35</v>
       </c>
@@ -4020,64 +4101,67 @@
       </c>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
+    <row r="63" spans="1:20" s="11" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="10">
         <v>2</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="10">
         <v>38.04</v>
       </c>
-      <c r="G63" s="2">
-        <v>0</v>
-      </c>
-      <c r="H63" s="2">
+      <c r="G63" s="10">
+        <v>0</v>
+      </c>
+      <c r="H63" s="10">
         <v>0.85</v>
       </c>
-      <c r="I63" s="2" t="b">
+      <c r="I63" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="J63" s="2">
-        <v>0</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L63" s="2">
+      <c r="J63" s="10">
+        <v>0</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L63" s="10">
         <v>2</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="10">
         <v>36.33</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="10">
         <v>36.94</v>
       </c>
-      <c r="O63" s="2">
+      <c r="O63" s="10">
         <v>-16.170000000000002</v>
       </c>
-      <c r="P63" s="2">
+      <c r="P63" s="10">
         <v>32.33</v>
       </c>
-      <c r="Q63" s="2">
-        <v>0</v>
-      </c>
-      <c r="R63" s="2">
-        <v>0</v>
-      </c>
-      <c r="S63" s="2">
+      <c r="Q63" s="10">
+        <v>0</v>
+      </c>
+      <c r="R63" s="10">
+        <v>0</v>
+      </c>
+      <c r="S63" s="10">
         <v>1</v>
       </c>
-      <c r="T63" s="2"/>
-    </row>
-    <row r="64" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="T63" s="10"/>
+    </row>
+    <row r="64" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>36</v>
       </c>
@@ -4134,7 +4218,7 @@
       </c>
       <c r="T64" s="2"/>
     </row>
-    <row r="65" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>36</v>
       </c>
@@ -4191,7 +4275,7 @@
       </c>
       <c r="T65" s="2"/>
     </row>
-    <row r="66" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>36</v>
       </c>
@@ -4248,7 +4332,7 @@
       </c>
       <c r="T66" s="2"/>
     </row>
-    <row r="67" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>36</v>
       </c>
@@ -4307,7 +4391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>36</v>
       </c>
@@ -4364,7 +4448,7 @@
       </c>
       <c r="T68" s="2"/>
     </row>
-    <row r="69" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>36</v>
       </c>
@@ -4421,7 +4505,7 @@
       </c>
       <c r="T69" s="2"/>
     </row>
-    <row r="70" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>36</v>
       </c>
@@ -4478,7 +4562,7 @@
       </c>
       <c r="T70" s="2"/>
     </row>
-    <row r="71" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>36</v>
       </c>
@@ -4535,7 +4619,7 @@
       </c>
       <c r="T71" s="2"/>
     </row>
-    <row r="72" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>36</v>
       </c>
@@ -4592,7 +4676,7 @@
       </c>
       <c r="T72" s="2"/>
     </row>
-    <row r="73" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>36</v>
       </c>
@@ -4649,7 +4733,7 @@
       </c>
       <c r="T73" s="2"/>
     </row>
-    <row r="74" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>36</v>
       </c>
@@ -4706,7 +4790,7 @@
       </c>
       <c r="T74" s="2"/>
     </row>
-    <row r="75" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
         <v>36</v>
       </c>
@@ -4763,7 +4847,7 @@
       </c>
       <c r="T75" s="2"/>
     </row>
-    <row r="76" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>36</v>
       </c>
@@ -4820,7 +4904,7 @@
       </c>
       <c r="T76" s="2"/>
     </row>
-    <row r="77" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>36</v>
       </c>
@@ -4877,7 +4961,7 @@
       </c>
       <c r="T77" s="2"/>
     </row>
-    <row r="78" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>36</v>
       </c>
@@ -4934,66 +5018,69 @@
       </c>
       <c r="T78" s="2"/>
     </row>
-    <row r="79" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
+    <row r="79" spans="1:20" s="11" customFormat="1" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="10">
         <v>4</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="10">
         <v>36.96</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="10">
         <v>1.17</v>
       </c>
-      <c r="H79" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J79" s="2">
+      <c r="H79" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" s="10">
         <v>0.17</v>
       </c>
-      <c r="K79" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L79" s="2">
+      <c r="K79" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L79" s="10">
         <v>4</v>
       </c>
-      <c r="M79" s="2">
+      <c r="M79" s="10">
         <v>28.96</v>
       </c>
-      <c r="N79" s="2">
+      <c r="N79" s="10">
         <v>30.17</v>
       </c>
-      <c r="O79" s="2">
+      <c r="O79" s="10">
         <v>-10.48</v>
       </c>
-      <c r="P79" s="2">
+      <c r="P79" s="10">
         <v>20.96</v>
       </c>
-      <c r="Q79" s="2">
+      <c r="Q79" s="10">
         <v>9.1199999999999992</v>
       </c>
-      <c r="R79" s="2">
+      <c r="R79" s="10">
         <v>2</v>
       </c>
-      <c r="S79" s="2">
+      <c r="S79" s="10">
         <v>0.01</v>
       </c>
-      <c r="T79" s="2" t="s">
+      <c r="T79" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>36</v>
       </c>
@@ -5050,7 +5137,7 @@
       </c>
       <c r="T80" s="2"/>
     </row>
-    <row r="81" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>36</v>
       </c>
@@ -5107,7 +5194,7 @@
       </c>
       <c r="T81" s="2"/>
     </row>
-    <row r="82" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>36</v>
       </c>
@@ -5164,7 +5251,7 @@
       </c>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>36</v>
       </c>
@@ -5221,7 +5308,7 @@
       </c>
       <c r="T83" s="2"/>
     </row>
-    <row r="84" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>36</v>
       </c>
@@ -5278,7 +5365,7 @@
       </c>
       <c r="T84" s="2"/>
     </row>
-    <row r="85" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>36</v>
       </c>
@@ -5335,7 +5422,7 @@
       </c>
       <c r="T85" s="2"/>
     </row>
-    <row r="86" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>36</v>
       </c>
@@ -5392,7 +5479,7 @@
       </c>
       <c r="T86" s="2"/>
     </row>
-    <row r="87" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>36</v>
       </c>
@@ -5449,7 +5536,7 @@
       </c>
       <c r="T87" s="2"/>
     </row>
-    <row r="88" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>36</v>
       </c>
@@ -5506,7 +5593,10 @@
       </c>
       <c r="T88" s="2"/>
     </row>
-    <row r="89" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="B89" s="2" t="s">
         <v>36</v>
       </c>
@@ -5563,7 +5653,7 @@
       </c>
       <c r="T89" s="2"/>
     </row>
-    <row r="90" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>36</v>
       </c>
@@ -5620,7 +5710,7 @@
       </c>
       <c r="T90" s="2"/>
     </row>
-    <row r="91" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>36</v>
       </c>
@@ -5677,7 +5767,7 @@
       </c>
       <c r="T91" s="2"/>
     </row>
-    <row r="92" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>36</v>
       </c>
@@ -5734,7 +5824,7 @@
       </c>
       <c r="T92" s="2"/>
     </row>
-    <row r="93" spans="2:20" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="15.65" x14ac:dyDescent="0.25">
       <c r="B93" s="3"/>
     </row>
   </sheetData>

</xml_diff>